<commit_message>
MergeSortVisualizer 사용으로 원상복귀 / Excel 업데이트
</commit_message>
<xml_diff>
--- a/성능 분석표.xlsx
+++ b/성능 분석표.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2b7ce060cadc8929/바탕 화면/2DGP/Sorts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="168" documentId="8_{ACCFC231-45CD-4983-AAEC-BCD5596D96A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{448F17F3-C20B-4FFD-9788-4EF17CFFFFEC}"/>
+  <xr:revisionPtr revIDLastSave="191" documentId="8_{ACCFC231-45CD-4983-AAEC-BCD5596D96A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC6C060F-C9D9-46D6-816F-F5C3B0D0A8A5}"/>
   <bookViews>
-    <workbookView xWindow="370" yWindow="320" windowWidth="15790" windowHeight="11170" xr2:uid="{E3B94454-7AC9-4D82-8668-599809F79E7C}"/>
+    <workbookView xWindow="-550" yWindow="910" windowWidth="15790" windowHeight="11170" xr2:uid="{E3B94454-7AC9-4D82-8668-599809F79E7C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Shell</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -53,6 +53,10 @@
   </si>
   <si>
     <t>Merge</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Merge-Ins</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -121,6 +125,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -440,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D05B0D5B-DF62-4A33-9737-8A12938F6FF0}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -451,7 +459,7 @@
     <col min="1" max="1" width="10.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -468,8 +476,11 @@
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>100</v>
       </c>
@@ -488,8 +499,11 @@
       <c r="F2" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>1000</v>
       </c>
@@ -508,8 +522,11 @@
       <c r="F3" s="1">
         <v>2E-3</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G3" s="1">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>2000</v>
       </c>
@@ -528,8 +545,11 @@
       <c r="F4" s="1">
         <v>3.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G4" s="1">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>3000</v>
       </c>
@@ -548,8 +568,11 @@
       <c r="F5" s="1">
         <v>5.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G5" s="1">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>4000</v>
       </c>
@@ -568,8 +591,11 @@
       <c r="F6" s="1">
         <v>7.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G6" s="1">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>5000</v>
       </c>
@@ -588,8 +614,11 @@
       <c r="F7" s="1">
         <v>2.1999999999999999E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G7" s="1">
+        <v>7.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>6000</v>
       </c>
@@ -608,8 +637,11 @@
       <c r="F8" s="1">
         <v>2.5999999999999999E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G8" s="1">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>7000</v>
       </c>
@@ -628,8 +660,11 @@
       <c r="F9" s="1">
         <v>2.3E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G9" s="1">
+        <v>1.2E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>8000</v>
       </c>
@@ -648,8 +683,11 @@
       <c r="F10" s="1">
         <v>2.9000000000000001E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G10" s="1">
+        <v>1.2E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>9000</v>
       </c>
@@ -668,8 +706,11 @@
       <c r="F11" s="1">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G11" s="1">
+        <v>1.7000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>10000</v>
       </c>
@@ -688,8 +729,11 @@
       <c r="F12" s="1">
         <v>3.2000000000000001E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G12" s="1">
+        <v>1.9E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>15000</v>
       </c>
@@ -708,8 +752,11 @@
       <c r="F13" s="1">
         <v>4.8000000000000001E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G13" s="1">
+        <v>2.9000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>20000</v>
       </c>
@@ -728,8 +775,11 @@
       <c r="F14" s="1">
         <v>7.3999999999999996E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G14" s="1">
+        <v>4.1000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>30000</v>
       </c>
@@ -748,8 +798,11 @@
       <c r="F15" s="1">
         <v>0.10299999999999999</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G15" s="1">
+        <v>6.9000000000000006E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>40000</v>
       </c>
@@ -768,8 +821,11 @@
       <c r="F16" s="1">
         <v>0.13300000000000001</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G16" s="1">
+        <v>9.7000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>50000</v>
       </c>
@@ -788,8 +844,11 @@
       <c r="F17" s="1">
         <v>0.17499999999999999</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G17" s="1">
+        <v>0.13200000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>100000</v>
       </c>
@@ -808,8 +867,11 @@
       <c r="F18" s="1">
         <v>0.36599999999999999</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G18" s="1">
+        <v>0.21199999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>200000</v>
       </c>
@@ -828,8 +890,11 @@
       <c r="F19" s="1">
         <v>0.68799999999999994</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G19" s="1">
+        <v>0.56399999999999995</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
         <v>300000</v>
       </c>
@@ -848,8 +913,11 @@
       <c r="F20" s="1">
         <v>0.96</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G20" s="1">
+        <v>0.80100000000000005</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="1">
         <v>400000</v>
       </c>
@@ -868,8 +936,11 @@
       <c r="F21" s="1">
         <v>1.552</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G21" s="1">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="1">
         <v>500000</v>
       </c>
@@ -888,8 +959,11 @@
       <c r="F22" s="1">
         <v>1.9850000000000001</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G22" s="1">
+        <v>1.6990000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="1">
         <v>1000000</v>
       </c>
@@ -901,8 +975,11 @@
       <c r="F23" s="1">
         <v>4.2839999999999998</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G23" s="1">
+        <v>3.2309999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
         <v>10000000</v>
       </c>

</xml_diff>